<commit_message>
Special items can now be nested.
</commit_message>
<xml_diff>
--- a/DynamicMarket.xlsx
+++ b/DynamicMarket.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Uni\WS21\kotlin\DynamicMarketKt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Personal\DynamicMarketKt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8055DDF4-28A2-4B7B-9C32-F6596F8B2846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DAA345-4C67-4BB1-A0FD-E6419C32DBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="9" r:id="rId1"/>
@@ -1850,8 +1850,8 @@
   </sheetPr>
   <dimension ref="A1:AL1025"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5524,8 +5524,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A267" sqref="A267"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="A263" sqref="A263:XFD263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12476,7 +12476,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>